<commit_message>
Updated referecne reveerse delete rules
</commit_message>
<xml_diff>
--- a/experiment_data/peritonitis_t_template.xlsx
+++ b/experiment_data/peritonitis_t_template.xlsx
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Pan gd PE-Cy5,Pan gd PECy5</t>
   </si>
   <si>
-    <t xml:space="preserve">.*CD\s*-*4\s.*$</t>
+    <t xml:space="preserve">.*CD\s*-*4$</t>
   </si>
   <si>
     <t xml:space="preserve">.*CD\s*-*27.*</t>
@@ -370,7 +370,7 @@
       <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
   </cols>
@@ -533,10 +533,10 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.79"/>

</xml_diff>